<commit_message>
EA PB awards now nominally working, did a build_cnc_update.bat to rebuild last 2 years from databases
</commit_message>
<xml_diff>
--- a/EA_PB_Awards_tables.xlsx
+++ b/EA_PB_Awards_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\powerof10-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6676096F-EE90-476C-AF2D-EAF5B2DEAFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CE0586-8306-4786-A2CB-6BDD254E75F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D5AEBD73-40BA-4FFC-A278-C286A81C8B58}"/>
   </bookViews>
@@ -2648,15 +2648,6 @@
     <t>Endurance</t>
   </si>
   <si>
-    <t>Sprint</t>
-  </si>
-  <si>
-    <t>Throw</t>
-  </si>
-  <si>
-    <t>Jump</t>
-  </si>
-  <si>
     <t>Combined</t>
   </si>
   <si>
@@ -2676,6 +2667,15 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Sprints</t>
+  </si>
+  <si>
+    <t>Jumps</t>
+  </si>
+  <si>
+    <t>Throws</t>
   </si>
 </sst>
 </file>
@@ -3083,8 +3083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDFC7DAF-7CF7-4414-A97B-3CF040F45606}">
   <dimension ref="A1:N387"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
-      <selection activeCell="C254" sqref="C254"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3145,7 +3145,7 @@
     </row>
     <row r="12" spans="1:14" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>251</v>
@@ -3189,7 +3189,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B13" s="3">
         <v>60</v>
@@ -3230,7 +3230,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B14" s="3">
         <v>60</v>
@@ -3271,7 +3271,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B15" s="3">
         <v>60</v>
@@ -3312,7 +3312,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B16" s="3">
         <v>60</v>
@@ -3353,7 +3353,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B17" s="3">
         <v>60</v>
@@ -3394,7 +3394,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B18" s="3">
         <v>75</v>
@@ -3435,7 +3435,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B19" s="3">
         <v>100</v>
@@ -3476,7 +3476,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B20" s="3">
         <v>100</v>
@@ -3517,7 +3517,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B21" s="3">
         <v>100</v>
@@ -3558,7 +3558,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B22" s="3">
         <v>100</v>
@@ -3599,7 +3599,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B23" s="3">
         <v>100</v>
@@ -3640,7 +3640,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B24" s="3">
         <v>150</v>
@@ -3681,7 +3681,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B25" s="3">
         <v>200</v>
@@ -3722,7 +3722,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B26" s="3">
         <v>200</v>
@@ -3763,7 +3763,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B27" s="3">
         <v>200</v>
@@ -3804,7 +3804,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B28" s="3">
         <v>200</v>
@@ -3845,7 +3845,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B29" s="3">
         <v>200</v>
@@ -3886,7 +3886,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B30" s="3">
         <v>300</v>
@@ -3927,7 +3927,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B31" s="3">
         <v>300</v>
@@ -3968,7 +3968,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B32" s="3">
         <v>300</v>
@@ -4009,7 +4009,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B33" s="3">
         <v>300</v>
@@ -4050,7 +4050,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B34" s="3">
         <v>400</v>
@@ -4091,7 +4091,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B35" s="3">
         <v>400</v>
@@ -4132,7 +4132,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B36" s="3">
         <v>400</v>
@@ -4173,7 +4173,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B37" s="3">
         <v>60</v>
@@ -4214,7 +4214,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B38" s="3">
         <v>60</v>
@@ -4255,7 +4255,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B39" s="3">
         <v>60</v>
@@ -4296,7 +4296,7 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B40" s="3">
         <v>60</v>
@@ -4337,7 +4337,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B41" s="3">
         <v>60</v>
@@ -4378,7 +4378,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B42" s="3">
         <v>75</v>
@@ -4419,7 +4419,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B43" s="3">
         <v>100</v>
@@ -4460,7 +4460,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B44" s="3">
         <v>100</v>
@@ -4501,7 +4501,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B45" s="3">
         <v>100</v>
@@ -4542,7 +4542,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B46" s="3">
         <v>100</v>
@@ -4583,7 +4583,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B47" s="3">
         <v>100</v>
@@ -4624,7 +4624,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B48" s="3">
         <v>150</v>
@@ -4665,7 +4665,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B49" s="3">
         <v>200</v>
@@ -4706,7 +4706,7 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B50" s="3">
         <v>200</v>
@@ -4747,7 +4747,7 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B51" s="3">
         <v>200</v>
@@ -4788,7 +4788,7 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B52" s="3">
         <v>200</v>
@@ -4829,7 +4829,7 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B53" s="3">
         <v>200</v>
@@ -4870,7 +4870,7 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B54" s="3">
         <v>300</v>
@@ -4911,7 +4911,7 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B55" s="3">
         <v>300</v>
@@ -4952,7 +4952,7 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B56" s="3">
         <v>300</v>
@@ -4993,7 +4993,7 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B57" s="3">
         <v>300</v>
@@ -5034,7 +5034,7 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B58" s="3">
         <v>400</v>
@@ -5075,7 +5075,7 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B59" s="3">
         <v>400</v>
@@ -5116,7 +5116,7 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>210</v>
@@ -5155,12 +5155,12 @@
         <v>1</v>
       </c>
       <c r="N60" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>211</v>
@@ -5201,7 +5201,7 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>212</v>
@@ -5242,7 +5242,7 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>213</v>
@@ -5283,7 +5283,7 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>202</v>
@@ -5324,7 +5324,7 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>205</v>
@@ -5365,7 +5365,7 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>206</v>
@@ -5406,7 +5406,7 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>207</v>
@@ -5447,7 +5447,7 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>208</v>
@@ -5488,7 +5488,7 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>203</v>
@@ -5529,7 +5529,7 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>209</v>
@@ -5570,7 +5570,7 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>204</v>
@@ -5611,7 +5611,7 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>204</v>
@@ -5652,7 +5652,7 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>215</v>
@@ -5693,7 +5693,7 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>214</v>
@@ -5734,7 +5734,7 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>216</v>
@@ -5775,7 +5775,7 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>217</v>
@@ -5816,7 +5816,7 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>217</v>
@@ -5857,7 +5857,7 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>218</v>
@@ -5898,7 +5898,7 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>219</v>
@@ -5939,7 +5939,7 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>220</v>
@@ -5980,7 +5980,7 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>221</v>
@@ -6021,7 +6021,7 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>221</v>
@@ -6062,7 +6062,7 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>223</v>
@@ -6103,7 +6103,7 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>222</v>
@@ -6144,7 +6144,7 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>222</v>
@@ -7743,7 +7743,7 @@
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>471</v>
@@ -7784,7 +7784,7 @@
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>472</v>
@@ -7825,7 +7825,7 @@
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>473</v>
@@ -7866,7 +7866,7 @@
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>474</v>
@@ -7907,7 +7907,7 @@
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>475</v>
@@ -7948,7 +7948,7 @@
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>476</v>
@@ -7989,7 +7989,7 @@
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>477</v>
@@ -8030,7 +8030,7 @@
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>479</v>
@@ -8071,7 +8071,7 @@
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>478</v>
@@ -8112,7 +8112,7 @@
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>480</v>
@@ -8153,7 +8153,7 @@
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>481</v>
@@ -8194,7 +8194,7 @@
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>482</v>
@@ -8235,7 +8235,7 @@
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B136" s="3" t="s">
         <v>483</v>
@@ -8276,7 +8276,7 @@
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>484</v>
@@ -8317,7 +8317,7 @@
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>485</v>
@@ -8358,7 +8358,7 @@
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>486</v>
@@ -8399,7 +8399,7 @@
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>487</v>
@@ -8440,7 +8440,7 @@
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>488</v>
@@ -8481,7 +8481,7 @@
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>488</v>
@@ -8522,7 +8522,7 @@
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>519</v>
@@ -8563,7 +8563,7 @@
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B144" s="3" t="s">
         <v>471</v>
@@ -8604,7 +8604,7 @@
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B145" s="3" t="s">
         <v>471</v>
@@ -8645,7 +8645,7 @@
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B146" s="3" t="s">
         <v>472</v>
@@ -8686,7 +8686,7 @@
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>472</v>
@@ -8727,7 +8727,7 @@
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>520</v>
@@ -8768,7 +8768,7 @@
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B149" s="3" t="s">
         <v>476</v>
@@ -8809,7 +8809,7 @@
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B150" s="3" t="s">
         <v>476</v>
@@ -8850,7 +8850,7 @@
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B151" s="3" t="s">
         <v>476</v>
@@ -8891,7 +8891,7 @@
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B152" s="3" t="s">
         <v>476</v>
@@ -8932,7 +8932,7 @@
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B153" s="3" t="s">
         <v>521</v>
@@ -8973,7 +8973,7 @@
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B154" s="3" t="s">
         <v>521</v>
@@ -9014,7 +9014,7 @@
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B155" s="3" t="s">
         <v>481</v>
@@ -9055,7 +9055,7 @@
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B156" s="3" t="s">
         <v>481</v>
@@ -9096,7 +9096,7 @@
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B157" s="3" t="s">
         <v>485</v>
@@ -9137,7 +9137,7 @@
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B158" s="3" t="s">
         <v>522</v>
@@ -9178,7 +9178,7 @@
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B159" s="3" t="s">
         <v>522</v>
@@ -9219,7 +9219,7 @@
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B160" s="3" t="s">
         <v>486</v>
@@ -9260,7 +9260,7 @@
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="B161" s="3" t="s">
         <v>486</v>
@@ -9301,7 +9301,7 @@
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B162" s="3" t="s">
         <v>574</v>
@@ -9342,7 +9342,7 @@
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B163" s="3" t="s">
         <v>574</v>
@@ -9383,7 +9383,7 @@
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B164" s="3" t="s">
         <v>574</v>
@@ -9424,7 +9424,7 @@
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B165" s="3" t="s">
         <v>574</v>
@@ -9465,7 +9465,7 @@
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B166" s="3" t="s">
         <v>574</v>
@@ -9506,7 +9506,7 @@
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B167" s="3" t="s">
         <v>575</v>
@@ -9547,7 +9547,7 @@
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B168" s="3" t="s">
         <v>575</v>
@@ -9588,7 +9588,7 @@
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B169" s="3" t="s">
         <v>575</v>
@@ -9629,7 +9629,7 @@
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B170" s="3" t="s">
         <v>575</v>
@@ -9670,7 +9670,7 @@
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B171" s="3" t="s">
         <v>576</v>
@@ -9711,7 +9711,7 @@
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B172" s="3" t="s">
         <v>576</v>
@@ -9752,7 +9752,7 @@
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B173" s="3" t="s">
         <v>576</v>
@@ -9793,7 +9793,7 @@
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B174" s="3" t="s">
         <v>576</v>
@@ -9834,7 +9834,7 @@
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B175" s="3" t="s">
         <v>576</v>
@@ -9875,7 +9875,7 @@
     </row>
     <row r="176" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B176" s="3" t="s">
         <v>577</v>
@@ -9916,7 +9916,7 @@
     </row>
     <row r="177" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B177" s="3" t="s">
         <v>577</v>
@@ -9957,7 +9957,7 @@
     </row>
     <row r="178" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B178" s="3" t="s">
         <v>577</v>
@@ -9998,7 +9998,7 @@
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B179" s="3" t="s">
         <v>577</v>
@@ -10039,7 +10039,7 @@
     </row>
     <row r="180" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B180" s="3" t="s">
         <v>574</v>
@@ -10080,7 +10080,7 @@
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B181" s="3" t="s">
         <v>574</v>
@@ -10121,7 +10121,7 @@
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B182" s="3" t="s">
         <v>574</v>
@@ -10162,7 +10162,7 @@
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B183" s="3" t="s">
         <v>574</v>
@@ -10203,7 +10203,7 @@
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B184" s="3" t="s">
         <v>574</v>
@@ -10244,7 +10244,7 @@
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B185" s="3" t="s">
         <v>575</v>
@@ -10285,7 +10285,7 @@
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B186" s="3" t="s">
         <v>575</v>
@@ -10326,7 +10326,7 @@
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B187" s="3" t="s">
         <v>575</v>
@@ -10367,7 +10367,7 @@
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B188" s="3" t="s">
         <v>575</v>
@@ -10408,7 +10408,7 @@
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B189" s="3" t="s">
         <v>576</v>
@@ -10449,7 +10449,7 @@
     </row>
     <row r="190" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B190" s="3" t="s">
         <v>576</v>
@@ -10490,7 +10490,7 @@
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B191" s="3" t="s">
         <v>576</v>
@@ -10531,7 +10531,7 @@
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B192" s="3" t="s">
         <v>576</v>
@@ -10572,7 +10572,7 @@
     </row>
     <row r="193" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B193" s="3" t="s">
         <v>576</v>
@@ -10613,7 +10613,7 @@
     </row>
     <row r="194" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B194" s="3" t="s">
         <v>577</v>
@@ -10654,7 +10654,7 @@
     </row>
     <row r="195" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B195" s="3" t="s">
         <v>577</v>
@@ -10695,7 +10695,7 @@
     </row>
     <row r="196" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B196" s="3" t="s">
         <v>577</v>
@@ -10736,7 +10736,7 @@
     </row>
     <row r="197" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>871</v>
+        <v>877</v>
       </c>
       <c r="B197" s="3" t="s">
         <v>577</v>
@@ -10777,7 +10777,7 @@
     </row>
     <row r="198" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="B198" s="3" t="s">
         <v>634</v>
@@ -10821,7 +10821,7 @@
     </row>
     <row r="199" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="B199" s="3" t="s">
         <v>635</v>
@@ -10862,7 +10862,7 @@
     </row>
     <row r="200" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="B200" s="3" t="s">
         <v>636</v>
@@ -10903,7 +10903,7 @@
     </row>
     <row r="201" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="B201" s="3" t="s">
         <v>637</v>
@@ -10944,7 +10944,7 @@
     </row>
     <row r="202" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="B202" s="3" t="s">
         <v>638</v>
@@ -10985,7 +10985,7 @@
     </row>
     <row r="203" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="B203" s="3" t="s">
         <v>628</v>
@@ -11027,7 +11027,7 @@
     </row>
     <row r="204" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="B204" s="3" t="s">
         <v>629</v>
@@ -11068,7 +11068,7 @@
     </row>
     <row r="205" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="B205" s="3" t="s">
         <v>630</v>
@@ -11109,7 +11109,7 @@
     </row>
     <row r="206" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="B206" s="3" t="s">
         <v>631</v>
@@ -11150,7 +11150,7 @@
     </row>
     <row r="207" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="B207" s="3" t="s">
         <v>632</v>
@@ -11191,7 +11191,7 @@
     </row>
     <row r="208" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="B208" s="3" t="s">
         <v>633</v>
@@ -11232,7 +11232,7 @@
     </row>
     <row r="209" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="B209" s="3" t="s">
         <v>641</v>
@@ -11276,7 +11276,7 @@
     </row>
     <row r="210" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="B210" s="3" t="s">
         <v>642</v>
@@ -11317,7 +11317,7 @@
     </row>
     <row r="211" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="B211" s="3" t="s">
         <v>643</v>
@@ -11358,7 +11358,7 @@
     </row>
     <row r="212" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="B212" s="3" t="s">
         <v>644</v>
@@ -11399,7 +11399,7 @@
     </row>
     <row r="213" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="B213" s="3" t="s">
         <v>644</v>
@@ -11440,7 +11440,7 @@
     </row>
     <row r="214" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="B214" s="3" t="s">
         <v>645</v>
@@ -11482,7 +11482,7 @@
     </row>
     <row r="215" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="B215" s="3" t="s">
         <v>646</v>
@@ -11523,7 +11523,7 @@
     </row>
     <row r="216" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="B216" s="3" t="s">
         <v>647</v>
@@ -11564,7 +11564,7 @@
     </row>
     <row r="217" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="B217" s="3" t="s">
         <v>648</v>
@@ -11605,7 +11605,7 @@
     </row>
     <row r="218" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="B218" s="3" t="s">
         <v>648</v>
@@ -11685,7 +11685,7 @@
         <v>657</v>
       </c>
       <c r="N219" s="3" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
     </row>
     <row r="220" spans="1:14" x14ac:dyDescent="0.25">
@@ -11852,7 +11852,7 @@
         <v>694</v>
       </c>
       <c r="N223" s="3" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
     </row>
     <row r="224" spans="1:14" x14ac:dyDescent="0.25">
@@ -12675,7 +12675,7 @@
         <v>793</v>
       </c>
       <c r="N243" s="3" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
     </row>
     <row r="244" spans="1:14" x14ac:dyDescent="0.25">
@@ -13014,7 +13014,7 @@
         <v>860</v>
       </c>
       <c r="C252" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="D252" t="s">
         <v>250</v>
@@ -13058,7 +13058,7 @@
         <v>861</v>
       </c>
       <c r="C253" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="D253" t="s">
         <v>250</v>

</xml_diff>